<commit_message>
gem rails admin and bundle
</commit_message>
<xml_diff>
--- a/Peanut.xlsx
+++ b/Peanut.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
   <si>
     <t>durée du crédit</t>
   </si>
@@ -71,12 +71,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="172" formatCode="#,##0.00000000\ &quot;€&quot;;[Red]\-#,##0.00000000\ &quot;€&quot;"/>
     <numFmt numFmtId="173" formatCode="0.0%"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00\ [$€-40C]_-;\-* #,##0.00\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0.000\ [$€-40C]_-;\-* #,##0.000\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-* #,##0.00000\ [$€-40C]_-;\-* #,##0.00000\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
   </numFmts>
@@ -129,7 +130,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -138,8 +139,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -155,16 +164,25 @@
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="16">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1484,16 +1502,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:Q3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="14" bestFit="1" customWidth="1"/>
@@ -1578,76 +1596,183 @@
       <c r="B3">
         <v>10000</v>
       </c>
-      <c r="C3" s="10">
-        <f>B3*$C6+B3</f>
+      <c r="C3" s="11">
+        <f>B3*$B6+B3</f>
         <v>10300</v>
       </c>
-      <c r="D3" s="10">
-        <f t="shared" ref="D3:G3" si="0">C3*$C6+C3</f>
+      <c r="D3" s="11">
+        <f>C3*$B6+C3</f>
         <v>10609</v>
       </c>
-      <c r="E3" s="10">
-        <f t="shared" si="0"/>
+      <c r="E3" s="11">
+        <f>D3*$B6+D3</f>
         <v>10927.27</v>
       </c>
-      <c r="F3" s="10">
-        <f t="shared" si="0"/>
+      <c r="F3" s="11">
+        <f>E3*$B6+E3</f>
         <v>11255.088100000001</v>
       </c>
-      <c r="G3" s="10">
-        <f t="shared" si="0"/>
+      <c r="G3" s="11">
+        <f>F3*$B6+F3</f>
         <v>11592.740743</v>
       </c>
-      <c r="H3" s="9">
-        <f>B3+B3*$H6</f>
+      <c r="H3" s="10">
+        <f>B3+B3*$C6</f>
         <v>10600</v>
       </c>
-      <c r="I3" s="9">
-        <f t="shared" ref="I3:L3" si="1">C3+C3*$H6</f>
+      <c r="I3" s="10">
+        <f>C3+C3*$C6</f>
         <v>10918</v>
       </c>
-      <c r="J3" s="9">
-        <f t="shared" si="1"/>
+      <c r="J3" s="10">
+        <f>D3+D3*$C6</f>
         <v>11245.54</v>
       </c>
-      <c r="K3" s="9">
-        <f t="shared" si="1"/>
+      <c r="K3" s="10">
+        <f>E3+E3*$C6</f>
         <v>11582.906200000001</v>
       </c>
-      <c r="L3" s="9">
-        <f t="shared" si="1"/>
+      <c r="L3" s="10">
+        <f>F3+F3*$C6</f>
         <v>11930.393386000002</v>
       </c>
-      <c r="M3" s="9">
-        <f>B3+B3*$M6</f>
+      <c r="M3" s="10">
+        <f>B3+B3*$D6</f>
         <v>10900</v>
       </c>
-      <c r="N3" s="9">
-        <f t="shared" ref="N3:Q3" si="2">C3+C3*$M6</f>
+      <c r="N3" s="10">
+        <f>C3+C3*$D6</f>
         <v>11227</v>
       </c>
-      <c r="O3" s="9">
-        <f t="shared" si="2"/>
+      <c r="O3" s="10">
+        <f>D3+D3*$D6</f>
         <v>11563.81</v>
       </c>
-      <c r="P3" s="9">
-        <f t="shared" si="2"/>
+      <c r="P3" s="10">
+        <f>E3+E3*$D6</f>
         <v>11910.7243</v>
       </c>
-      <c r="Q3" s="9">
-        <f t="shared" si="2"/>
+      <c r="Q3" s="10">
+        <f>F3+F3*$D6</f>
         <v>12268.046029000001</v>
       </c>
     </row>
     <row r="6" spans="1:17">
+      <c r="B6" s="8">
+        <v>0.03</v>
+      </c>
       <c r="C6" s="8">
-        <v>0.03</v>
-      </c>
-      <c r="H6" s="8">
         <v>0.06</v>
       </c>
-      <c r="M6" s="8">
+      <c r="D6" s="8">
         <v>0.09</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="B9" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C9" s="3">
+        <v>10000</v>
+      </c>
+      <c r="D9" s="3">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="9">
+        <f>B9*B$6+B9</f>
+        <v>10300</v>
+      </c>
+      <c r="C10" s="9">
+        <f t="shared" ref="C10:D14" si="0">C9*C$6+C9</f>
+        <v>10600</v>
+      </c>
+      <c r="D10" s="9">
+        <f t="shared" si="0"/>
+        <v>16350</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="9">
+        <f t="shared" ref="B11:B14" si="1">B10*B$6+B10</f>
+        <v>10609</v>
+      </c>
+      <c r="C11" s="9">
+        <f t="shared" si="0"/>
+        <v>11236</v>
+      </c>
+      <c r="D11" s="9">
+        <f t="shared" si="0"/>
+        <v>17821.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="9">
+        <f t="shared" si="1"/>
+        <v>10927.27</v>
+      </c>
+      <c r="C12" s="9">
+        <f t="shared" si="0"/>
+        <v>11910.16</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" si="0"/>
+        <v>19425.435000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="9">
+        <f t="shared" si="1"/>
+        <v>11255.088100000001</v>
+      </c>
+      <c r="C13" s="9">
+        <f t="shared" si="0"/>
+        <v>12624.7696</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" si="0"/>
+        <v>21173.724150000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="9">
+        <f t="shared" si="1"/>
+        <v>11592.740743</v>
+      </c>
+      <c r="C14" s="9">
+        <f t="shared" si="0"/>
+        <v>13382.255776</v>
+      </c>
+      <c r="D14" s="9">
+        <f t="shared" si="0"/>
+        <v>23079.359323500001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>